<commit_message>
Added minuses to attendance and made broj_izostanka accurate
</commit_message>
<xml_diff>
--- a/documents/NovaEvidencija.xlsx
+++ b/documents/NovaEvidencija.xlsx
@@ -753,8 +753,16 @@
           <t>Antonio Lipovac</t>
         </is>
       </c>
-      <c r="B3" s="5" t="n"/>
-      <c r="C3" s="5" t="n"/>
+      <c r="B3" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C3" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
       <c r="D3" s="5" t="inlineStr">
         <is>
           <t>+</t>
@@ -770,7 +778,11 @@
           <t>+</t>
         </is>
       </c>
-      <c r="G3" s="5" t="n"/>
+      <c r="G3" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
       <c r="H3" s="5" t="inlineStr">
         <is>
           <t>+</t>
@@ -821,7 +833,11 @@
           <t>+</t>
         </is>
       </c>
-      <c r="G4" s="5" t="n"/>
+      <c r="G4" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
       <c r="H4" s="5" t="inlineStr">
         <is>
           <t>+</t>
@@ -847,7 +863,11 @@
           <t>Antonio Muža</t>
         </is>
       </c>
-      <c r="B5" s="5" t="n"/>
+      <c r="B5" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
       <c r="C5" s="5" t="inlineStr">
         <is>
           <t>+</t>
@@ -858,9 +878,21 @@
           <t>+</t>
         </is>
       </c>
-      <c r="E5" s="5" t="n"/>
-      <c r="F5" s="5" t="n"/>
-      <c r="G5" s="5" t="n"/>
+      <c r="E5" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F5" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G5" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
       <c r="H5" s="5" t="inlineStr">
         <is>
           <t>+</t>
@@ -886,8 +918,16 @@
           <t>Bartol Matolić</t>
         </is>
       </c>
-      <c r="B6" s="5" t="n"/>
-      <c r="C6" s="5" t="n"/>
+      <c r="B6" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C6" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
       <c r="D6" s="5" t="inlineStr">
         <is>
           <t>+</t>
@@ -933,7 +973,11 @@
           <t>Bruno Matušić</t>
         </is>
       </c>
-      <c r="B7" s="5" t="n"/>
+      <c r="B7" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
       <c r="C7" s="5" t="inlineStr">
         <is>
           <t>+</t>
@@ -984,13 +1028,41 @@
           <t>Filip Boban</t>
         </is>
       </c>
-      <c r="B8" s="5" t="n"/>
-      <c r="C8" s="5" t="n"/>
-      <c r="D8" s="5" t="n"/>
-      <c r="E8" s="5" t="n"/>
-      <c r="F8" s="5" t="n"/>
-      <c r="G8" s="5" t="n"/>
-      <c r="H8" s="5" t="n"/>
+      <c r="B8" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C8" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D8" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E8" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F8" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G8" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H8" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
       <c r="I8" s="5" t="n"/>
       <c r="J8" s="5" t="n"/>
       <c r="K8" s="5" t="n"/>
@@ -1071,7 +1143,11 @@
           <t>+</t>
         </is>
       </c>
-      <c r="C10" s="5" t="n"/>
+      <c r="C10" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
       <c r="D10" s="5" t="inlineStr">
         <is>
           <t>+</t>
@@ -1087,8 +1163,16 @@
           <t>+</t>
         </is>
       </c>
-      <c r="G10" s="5" t="n"/>
-      <c r="H10" s="5" t="n"/>
+      <c r="G10" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H10" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
       <c r="I10" s="5" t="n"/>
       <c r="J10" s="5" t="n"/>
       <c r="K10" s="5" t="n"/>
@@ -1164,13 +1248,41 @@
           <t>Ivan Plećaš</t>
         </is>
       </c>
-      <c r="B12" s="5" t="n"/>
-      <c r="C12" s="5" t="n"/>
-      <c r="D12" s="5" t="n"/>
-      <c r="E12" s="5" t="n"/>
-      <c r="F12" s="5" t="n"/>
-      <c r="G12" s="5" t="n"/>
-      <c r="H12" s="5" t="n"/>
+      <c r="B12" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C12" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D12" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E12" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F12" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G12" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H12" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
       <c r="I12" s="5" t="n"/>
       <c r="J12" s="5" t="n"/>
       <c r="K12" s="5" t="n"/>
@@ -1191,16 +1303,36 @@
           <t>Juraj Tomiša</t>
         </is>
       </c>
-      <c r="B13" s="5" t="n"/>
-      <c r="C13" s="5" t="n"/>
+      <c r="B13" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C13" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
       <c r="D13" s="5" t="inlineStr">
         <is>
           <t>+</t>
         </is>
       </c>
-      <c r="E13" s="5" t="n"/>
-      <c r="F13" s="5" t="n"/>
-      <c r="G13" s="5" t="n"/>
+      <c r="E13" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F13" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G13" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
       <c r="H13" s="5" t="inlineStr">
         <is>
           <t>+</t>
@@ -1226,13 +1358,41 @@
           <t>Karlo Gardijan</t>
         </is>
       </c>
-      <c r="B14" s="5" t="n"/>
-      <c r="C14" s="5" t="n"/>
-      <c r="D14" s="5" t="n"/>
-      <c r="E14" s="5" t="n"/>
-      <c r="F14" s="5" t="n"/>
-      <c r="G14" s="5" t="n"/>
-      <c r="H14" s="5" t="n"/>
+      <c r="B14" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C14" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D14" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E14" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F14" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G14" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H14" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
       <c r="I14" s="5" t="n"/>
       <c r="J14" s="5" t="n"/>
       <c r="K14" s="5" t="n"/>
@@ -1308,7 +1468,11 @@
           <t>Lovro Rozman</t>
         </is>
       </c>
-      <c r="B16" s="5" t="n"/>
+      <c r="B16" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
       <c r="C16" s="5" t="inlineStr">
         <is>
           <t>+</t>
@@ -1319,9 +1483,21 @@
           <t>+</t>
         </is>
       </c>
-      <c r="E16" s="5" t="n"/>
-      <c r="F16" s="5" t="n"/>
-      <c r="G16" s="5" t="n"/>
+      <c r="E16" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F16" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G16" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
       <c r="H16" s="5" t="inlineStr">
         <is>
           <t>+</t>
@@ -1347,7 +1523,11 @@
           <t>Luka Mikulić</t>
         </is>
       </c>
-      <c r="B17" s="5" t="n"/>
+      <c r="B17" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
       <c r="C17" s="5" t="inlineStr">
         <is>
           <t>+</t>
@@ -1398,8 +1578,16 @@
           <t>Marin Plastić</t>
         </is>
       </c>
-      <c r="B18" s="5" t="n"/>
-      <c r="C18" s="5" t="n"/>
+      <c r="B18" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C18" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
       <c r="D18" s="5" t="inlineStr">
         <is>
           <t>+</t>
@@ -1410,8 +1598,16 @@
           <t>+</t>
         </is>
       </c>
-      <c r="F18" s="5" t="n"/>
-      <c r="G18" s="5" t="n"/>
+      <c r="F18" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G18" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
       <c r="H18" s="5" t="inlineStr">
         <is>
           <t>+</t>
@@ -1437,13 +1633,21 @@
           <t>Matija Dokmanović</t>
         </is>
       </c>
-      <c r="B19" s="5" t="n"/>
+      <c r="B19" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
       <c r="C19" s="5" t="inlineStr">
         <is>
           <t>+</t>
         </is>
       </c>
-      <c r="D19" s="5" t="n"/>
+      <c r="D19" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
       <c r="E19" s="5" t="inlineStr">
         <is>
           <t>+</t>
@@ -1459,7 +1663,11 @@
           <t>+</t>
         </is>
       </c>
-      <c r="H19" s="5" t="n"/>
+      <c r="H19" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
       <c r="I19" s="5" t="n"/>
       <c r="J19" s="5" t="n"/>
       <c r="K19" s="5" t="n"/>
@@ -1480,17 +1688,41 @@
           <t>Niki Hercigonja</t>
         </is>
       </c>
-      <c r="B20" s="5" t="n"/>
-      <c r="C20" s="5" t="n"/>
+      <c r="B20" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C20" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
       <c r="D20" s="5" t="inlineStr">
         <is>
           <t>+</t>
         </is>
       </c>
-      <c r="E20" s="5" t="n"/>
-      <c r="F20" s="5" t="n"/>
-      <c r="G20" s="5" t="n"/>
-      <c r="H20" s="5" t="n"/>
+      <c r="E20" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F20" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G20" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H20" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
       <c r="I20" s="5" t="n"/>
       <c r="J20" s="5" t="n"/>
       <c r="K20" s="5" t="n"/>
@@ -1511,13 +1743,21 @@
           <t>Niko Ivanić</t>
         </is>
       </c>
-      <c r="B21" s="5" t="n"/>
+      <c r="B21" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
       <c r="C21" s="5" t="inlineStr">
         <is>
           <t>+</t>
         </is>
       </c>
-      <c r="D21" s="5" t="n"/>
+      <c r="D21" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
       <c r="E21" s="5" t="inlineStr">
         <is>
           <t>+</t>
@@ -1533,7 +1773,11 @@
           <t>+</t>
         </is>
       </c>
-      <c r="H21" s="5" t="n"/>
+      <c r="H21" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
       <c r="I21" s="5" t="n"/>
       <c r="J21" s="5" t="n"/>
       <c r="K21" s="5" t="n"/>
@@ -1564,7 +1808,11 @@
           <t>+</t>
         </is>
       </c>
-      <c r="D22" s="5" t="n"/>
+      <c r="D22" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
       <c r="E22" s="5" t="inlineStr">
         <is>
           <t>+</t>
@@ -1580,7 +1828,11 @@
           <t>+</t>
         </is>
       </c>
-      <c r="H22" s="5" t="n"/>
+      <c r="H22" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
       <c r="I22" s="5" t="n"/>
       <c r="J22" s="5" t="n"/>
       <c r="K22" s="5" t="n"/>
@@ -1626,8 +1878,16 @@
           <t>+</t>
         </is>
       </c>
-      <c r="G23" s="5" t="n"/>
-      <c r="H23" s="5" t="n"/>
+      <c r="G23" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H23" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
       <c r="I23" s="5" t="n"/>
       <c r="J23" s="5" t="n"/>
       <c r="K23" s="5" t="n"/>
@@ -1648,7 +1908,11 @@
           <t>Patrik Kosor</t>
         </is>
       </c>
-      <c r="B24" s="5" t="n"/>
+      <c r="B24" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
       <c r="C24" s="5" t="inlineStr">
         <is>
           <t>+</t>
@@ -1724,7 +1988,11 @@
           <t>+</t>
         </is>
       </c>
-      <c r="G25" s="5" t="n"/>
+      <c r="G25" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
       <c r="H25" s="5" t="inlineStr">
         <is>
           <t>+</t>
@@ -1760,7 +2028,11 @@
           <t>+</t>
         </is>
       </c>
-      <c r="D26" s="5" t="n"/>
+      <c r="D26" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
       <c r="E26" s="5" t="inlineStr">
         <is>
           <t>+</t>
@@ -1801,20 +2073,36 @@
           <t>Sven Olah</t>
         </is>
       </c>
-      <c r="B27" s="5" t="n"/>
-      <c r="C27" s="5" t="n"/>
+      <c r="B27" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C27" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
       <c r="D27" s="5" t="inlineStr">
         <is>
           <t>+</t>
         </is>
       </c>
-      <c r="E27" s="5" t="n"/>
+      <c r="E27" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
       <c r="F27" s="5" t="inlineStr">
         <is>
           <t>+</t>
         </is>
       </c>
-      <c r="G27" s="5" t="n"/>
+      <c r="G27" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
       <c r="H27" s="5" t="inlineStr">
         <is>
           <t>+</t>
@@ -1850,15 +2138,31 @@
           <t>+</t>
         </is>
       </c>
-      <c r="D28" s="5" t="n"/>
+      <c r="D28" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
       <c r="E28" s="5" t="inlineStr">
         <is>
           <t>+</t>
         </is>
       </c>
-      <c r="F28" s="5" t="n"/>
-      <c r="G28" s="5" t="n"/>
-      <c r="H28" s="5" t="n"/>
+      <c r="F28" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G28" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H28" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
       <c r="I28" s="5" t="n"/>
       <c r="J28" s="5" t="n"/>
       <c r="K28" s="5" t="n"/>
@@ -1879,8 +2183,16 @@
           <t>Šimun Barberić</t>
         </is>
       </c>
-      <c r="B29" s="5" t="n"/>
-      <c r="C29" s="5" t="n"/>
+      <c r="B29" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C29" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
       <c r="D29" s="5" t="inlineStr">
         <is>
           <t>+</t>
@@ -1896,7 +2208,11 @@
           <t>+</t>
         </is>
       </c>
-      <c r="G29" s="5" t="n"/>
+      <c r="G29" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
       <c r="H29" s="5" t="inlineStr">
         <is>
           <t>+</t>
@@ -1932,7 +2248,11 @@
           <t>+</t>
         </is>
       </c>
-      <c r="D30" s="5" t="n"/>
+      <c r="D30" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
       <c r="E30" s="5" t="inlineStr">
         <is>
           <t>+</t>
@@ -1973,16 +2293,36 @@
           <t>Matej Desanić</t>
         </is>
       </c>
-      <c r="B31" s="5" t="n"/>
-      <c r="C31" s="5" t="n"/>
-      <c r="D31" s="5" t="n"/>
-      <c r="E31" s="5" t="n"/>
+      <c r="B31" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C31" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D31" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E31" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
       <c r="F31" s="5" t="inlineStr">
         <is>
           <t>+</t>
         </is>
       </c>
-      <c r="G31" s="5" t="n"/>
+      <c r="G31" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
       <c r="H31" s="5" t="inlineStr">
         <is>
           <t>+</t>
@@ -2003,14 +2343,46 @@
       <c r="U31" s="6" t="n"/>
     </row>
     <row r="32" ht="16.5" customHeight="1">
-      <c r="A32" s="4" t="n"/>
-      <c r="B32" s="5" t="n"/>
-      <c r="C32" s="5" t="n"/>
-      <c r="D32" s="5" t="n"/>
-      <c r="E32" s="5" t="n"/>
-      <c r="F32" s="5" t="n"/>
-      <c r="G32" s="5" t="n"/>
-      <c r="H32" s="5" t="n"/>
+      <c r="A32" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="B32" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C32" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D32" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E32" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F32" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G32" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H32" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
       <c r="I32" s="5" t="n"/>
       <c r="J32" s="5" t="n"/>
       <c r="K32" s="5" t="n"/>
@@ -2026,14 +2398,46 @@
       <c r="U32" s="6" t="n"/>
     </row>
     <row r="33" ht="16.5" customHeight="1">
-      <c r="A33" s="4" t="n"/>
-      <c r="B33" s="5" t="n"/>
-      <c r="C33" s="5" t="n"/>
-      <c r="D33" s="5" t="n"/>
-      <c r="E33" s="5" t="n"/>
-      <c r="F33" s="5" t="n"/>
-      <c r="G33" s="5" t="n"/>
-      <c r="H33" s="5" t="n"/>
+      <c r="A33" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="B33" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C33" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D33" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E33" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F33" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G33" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H33" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
       <c r="I33" s="5" t="n"/>
       <c r="J33" s="5" t="n"/>
       <c r="K33" s="5" t="n"/>
@@ -2049,14 +2453,46 @@
       <c r="U33" s="6" t="n"/>
     </row>
     <row r="34" ht="16.5" customHeight="1">
-      <c r="A34" s="4" t="n"/>
-      <c r="B34" s="5" t="n"/>
-      <c r="C34" s="5" t="n"/>
-      <c r="D34" s="5" t="n"/>
-      <c r="E34" s="5" t="n"/>
-      <c r="F34" s="5" t="n"/>
-      <c r="G34" s="5" t="n"/>
-      <c r="H34" s="5" t="n"/>
+      <c r="A34" s="4" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="B34" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C34" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D34" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E34" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F34" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G34" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H34" s="5" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
       <c r="I34" s="5" t="n"/>
       <c r="J34" s="5" t="n"/>
       <c r="K34" s="5" t="n"/>
@@ -2072,14 +2508,46 @@
       <c r="U34" s="6" t="n"/>
     </row>
     <row r="35" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A35" s="8" t="n"/>
-      <c r="B35" s="9" t="n"/>
-      <c r="C35" s="9" t="n"/>
-      <c r="D35" s="9" t="n"/>
-      <c r="E35" s="9" t="n"/>
-      <c r="F35" s="9" t="n"/>
-      <c r="G35" s="9" t="n"/>
-      <c r="H35" s="9" t="n"/>
+      <c r="A35" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="B35" s="9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="C35" s="9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D35" s="9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E35" s="9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="F35" s="9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="G35" s="9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="H35" s="9" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
       <c r="I35" s="9" t="n"/>
       <c r="J35" s="9" t="n"/>
       <c r="K35" s="9" t="n"/>

</xml_diff>